<commit_message>
adding for sand env
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ_SAND/Data/Template.xlsx
+++ b/Projects/LIONNZ_SAND/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -33,13 +33,16 @@
     <t xml:space="preserve">active</t>
   </si>
   <si>
-    <t xml:space="preserve">FSOS_OWN_MAN_ALL_SCENETYPE</t>
+    <t xml:space="preserve">FSOS_OWN_MANUFACTURER_IN_WHOLE_STORE</t>
   </si>
   <si>
     <t xml:space="preserve">FSOS</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOS_OWN_MAN_ALL_SCENETYPE</t>
   </si>
   <si>
     <t xml:space="preserve">FSOS_ALL_MAN_ALL_SCENETYPE</t>
@@ -114,13 +117,16 @@
     <t xml:space="preserve">manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">scene_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lion</t>
   </si>
   <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
     <t xml:space="preserve">off premise, on premise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_type</t>
   </si>
   <si>
     <t xml:space="preserve">brand</t>
@@ -130,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
   </si>
   <si>
     <t xml:space="preserve">Beer Tap</t>
@@ -292,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -331,10 +334,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -474,19 +473,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.5408163265306"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
@@ -511,7 +511,6 @@
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -544,7 +543,7 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3"/>
@@ -584,12 +583,10 @@
       <c r="D9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
@@ -597,18 +594,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -625,71 +634,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMH11"/>
+  <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topRight" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="57.5051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="47.3928571428572"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="67.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="8" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="0"/>
       <c r="P1" s="0"/>
@@ -1701,35 +1714,33 @@
       <c r="AMH1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="11" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="M2" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="N2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O2" s="0"/>
       <c r="P2" s="0"/>
@@ -2741,35 +2752,37 @@
       <c r="AMH2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
       <c r="K3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
@@ -3781,273 +3794,1313 @@
       <c r="AMH3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
+      <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
+      <c r="IX4" s="0"/>
+      <c r="IY4" s="0"/>
+      <c r="IZ4" s="0"/>
+      <c r="JA4" s="0"/>
+      <c r="JB4" s="0"/>
+      <c r="JC4" s="0"/>
+      <c r="JD4" s="0"/>
+      <c r="JE4" s="0"/>
+      <c r="JF4" s="0"/>
+      <c r="JG4" s="0"/>
+      <c r="JH4" s="0"/>
+      <c r="JI4" s="0"/>
+      <c r="JJ4" s="0"/>
+      <c r="JK4" s="0"/>
+      <c r="JL4" s="0"/>
+      <c r="JM4" s="0"/>
+      <c r="JN4" s="0"/>
+      <c r="JO4" s="0"/>
+      <c r="JP4" s="0"/>
+      <c r="JQ4" s="0"/>
+      <c r="JR4" s="0"/>
+      <c r="JS4" s="0"/>
+      <c r="JT4" s="0"/>
+      <c r="JU4" s="0"/>
+      <c r="JV4" s="0"/>
+      <c r="JW4" s="0"/>
+      <c r="JX4" s="0"/>
+      <c r="JY4" s="0"/>
+      <c r="JZ4" s="0"/>
+      <c r="KA4" s="0"/>
+      <c r="KB4" s="0"/>
+      <c r="KC4" s="0"/>
+      <c r="KD4" s="0"/>
+      <c r="KE4" s="0"/>
+      <c r="KF4" s="0"/>
+      <c r="KG4" s="0"/>
+      <c r="KH4" s="0"/>
+      <c r="KI4" s="0"/>
+      <c r="KJ4" s="0"/>
+      <c r="KK4" s="0"/>
+      <c r="KL4" s="0"/>
+      <c r="KM4" s="0"/>
+      <c r="KN4" s="0"/>
+      <c r="KO4" s="0"/>
+      <c r="KP4" s="0"/>
+      <c r="KQ4" s="0"/>
+      <c r="KR4" s="0"/>
+      <c r="KS4" s="0"/>
+      <c r="KT4" s="0"/>
+      <c r="KU4" s="0"/>
+      <c r="KV4" s="0"/>
+      <c r="KW4" s="0"/>
+      <c r="KX4" s="0"/>
+      <c r="KY4" s="0"/>
+      <c r="KZ4" s="0"/>
+      <c r="LA4" s="0"/>
+      <c r="LB4" s="0"/>
+      <c r="LC4" s="0"/>
+      <c r="LD4" s="0"/>
+      <c r="LE4" s="0"/>
+      <c r="LF4" s="0"/>
+      <c r="LG4" s="0"/>
+      <c r="LH4" s="0"/>
+      <c r="LI4" s="0"/>
+      <c r="LJ4" s="0"/>
+      <c r="LK4" s="0"/>
+      <c r="LL4" s="0"/>
+      <c r="LM4" s="0"/>
+      <c r="LN4" s="0"/>
+      <c r="LO4" s="0"/>
+      <c r="LP4" s="0"/>
+      <c r="LQ4" s="0"/>
+      <c r="LR4" s="0"/>
+      <c r="LS4" s="0"/>
+      <c r="LT4" s="0"/>
+      <c r="LU4" s="0"/>
+      <c r="LV4" s="0"/>
+      <c r="LW4" s="0"/>
+      <c r="LX4" s="0"/>
+      <c r="LY4" s="0"/>
+      <c r="LZ4" s="0"/>
+      <c r="MA4" s="0"/>
+      <c r="MB4" s="0"/>
+      <c r="MC4" s="0"/>
+      <c r="MD4" s="0"/>
+      <c r="ME4" s="0"/>
+      <c r="MF4" s="0"/>
+      <c r="MG4" s="0"/>
+      <c r="MH4" s="0"/>
+      <c r="MI4" s="0"/>
+      <c r="MJ4" s="0"/>
+      <c r="MK4" s="0"/>
+      <c r="ML4" s="0"/>
+      <c r="MM4" s="0"/>
+      <c r="MN4" s="0"/>
+      <c r="MO4" s="0"/>
+      <c r="MP4" s="0"/>
+      <c r="MQ4" s="0"/>
+      <c r="MR4" s="0"/>
+      <c r="MS4" s="0"/>
+      <c r="MT4" s="0"/>
+      <c r="MU4" s="0"/>
+      <c r="MV4" s="0"/>
+      <c r="MW4" s="0"/>
+      <c r="MX4" s="0"/>
+      <c r="MY4" s="0"/>
+      <c r="MZ4" s="0"/>
+      <c r="NA4" s="0"/>
+      <c r="NB4" s="0"/>
+      <c r="NC4" s="0"/>
+      <c r="ND4" s="0"/>
+      <c r="NE4" s="0"/>
+      <c r="NF4" s="0"/>
+      <c r="NG4" s="0"/>
+      <c r="NH4" s="0"/>
+      <c r="NI4" s="0"/>
+      <c r="NJ4" s="0"/>
+      <c r="NK4" s="0"/>
+      <c r="NL4" s="0"/>
+      <c r="NM4" s="0"/>
+      <c r="NN4" s="0"/>
+      <c r="NO4" s="0"/>
+      <c r="NP4" s="0"/>
+      <c r="NQ4" s="0"/>
+      <c r="NR4" s="0"/>
+      <c r="NS4" s="0"/>
+      <c r="NT4" s="0"/>
+      <c r="NU4" s="0"/>
+      <c r="NV4" s="0"/>
+      <c r="NW4" s="0"/>
+      <c r="NX4" s="0"/>
+      <c r="NY4" s="0"/>
+      <c r="NZ4" s="0"/>
+      <c r="OA4" s="0"/>
+      <c r="OB4" s="0"/>
+      <c r="OC4" s="0"/>
+      <c r="OD4" s="0"/>
+      <c r="OE4" s="0"/>
+      <c r="OF4" s="0"/>
+      <c r="OG4" s="0"/>
+      <c r="OH4" s="0"/>
+      <c r="OI4" s="0"/>
+      <c r="OJ4" s="0"/>
+      <c r="OK4" s="0"/>
+      <c r="OL4" s="0"/>
+      <c r="OM4" s="0"/>
+      <c r="ON4" s="0"/>
+      <c r="OO4" s="0"/>
+      <c r="OP4" s="0"/>
+      <c r="OQ4" s="0"/>
+      <c r="OR4" s="0"/>
+      <c r="OS4" s="0"/>
+      <c r="OT4" s="0"/>
+      <c r="OU4" s="0"/>
+      <c r="OV4" s="0"/>
+      <c r="OW4" s="0"/>
+      <c r="OX4" s="0"/>
+      <c r="OY4" s="0"/>
+      <c r="OZ4" s="0"/>
+      <c r="PA4" s="0"/>
+      <c r="PB4" s="0"/>
+      <c r="PC4" s="0"/>
+      <c r="PD4" s="0"/>
+      <c r="PE4" s="0"/>
+      <c r="PF4" s="0"/>
+      <c r="PG4" s="0"/>
+      <c r="PH4" s="0"/>
+      <c r="PI4" s="0"/>
+      <c r="PJ4" s="0"/>
+      <c r="PK4" s="0"/>
+      <c r="PL4" s="0"/>
+      <c r="PM4" s="0"/>
+      <c r="PN4" s="0"/>
+      <c r="PO4" s="0"/>
+      <c r="PP4" s="0"/>
+      <c r="PQ4" s="0"/>
+      <c r="PR4" s="0"/>
+      <c r="PS4" s="0"/>
+      <c r="PT4" s="0"/>
+      <c r="PU4" s="0"/>
+      <c r="PV4" s="0"/>
+      <c r="PW4" s="0"/>
+      <c r="PX4" s="0"/>
+      <c r="PY4" s="0"/>
+      <c r="PZ4" s="0"/>
+      <c r="QA4" s="0"/>
+      <c r="QB4" s="0"/>
+      <c r="QC4" s="0"/>
+      <c r="QD4" s="0"/>
+      <c r="QE4" s="0"/>
+      <c r="QF4" s="0"/>
+      <c r="QG4" s="0"/>
+      <c r="QH4" s="0"/>
+      <c r="QI4" s="0"/>
+      <c r="QJ4" s="0"/>
+      <c r="QK4" s="0"/>
+      <c r="QL4" s="0"/>
+      <c r="QM4" s="0"/>
+      <c r="QN4" s="0"/>
+      <c r="QO4" s="0"/>
+      <c r="QP4" s="0"/>
+      <c r="QQ4" s="0"/>
+      <c r="QR4" s="0"/>
+      <c r="QS4" s="0"/>
+      <c r="QT4" s="0"/>
+      <c r="QU4" s="0"/>
+      <c r="QV4" s="0"/>
+      <c r="QW4" s="0"/>
+      <c r="QX4" s="0"/>
+      <c r="QY4" s="0"/>
+      <c r="QZ4" s="0"/>
+      <c r="RA4" s="0"/>
+      <c r="RB4" s="0"/>
+      <c r="RC4" s="0"/>
+      <c r="RD4" s="0"/>
+      <c r="RE4" s="0"/>
+      <c r="RF4" s="0"/>
+      <c r="RG4" s="0"/>
+      <c r="RH4" s="0"/>
+      <c r="RI4" s="0"/>
+      <c r="RJ4" s="0"/>
+      <c r="RK4" s="0"/>
+      <c r="RL4" s="0"/>
+      <c r="RM4" s="0"/>
+      <c r="RN4" s="0"/>
+      <c r="RO4" s="0"/>
+      <c r="RP4" s="0"/>
+      <c r="RQ4" s="0"/>
+      <c r="RR4" s="0"/>
+      <c r="RS4" s="0"/>
+      <c r="RT4" s="0"/>
+      <c r="RU4" s="0"/>
+      <c r="RV4" s="0"/>
+      <c r="RW4" s="0"/>
+      <c r="RX4" s="0"/>
+      <c r="RY4" s="0"/>
+      <c r="RZ4" s="0"/>
+      <c r="SA4" s="0"/>
+      <c r="SB4" s="0"/>
+      <c r="SC4" s="0"/>
+      <c r="SD4" s="0"/>
+      <c r="SE4" s="0"/>
+      <c r="SF4" s="0"/>
+      <c r="SG4" s="0"/>
+      <c r="SH4" s="0"/>
+      <c r="SI4" s="0"/>
+      <c r="SJ4" s="0"/>
+      <c r="SK4" s="0"/>
+      <c r="SL4" s="0"/>
+      <c r="SM4" s="0"/>
+      <c r="SN4" s="0"/>
+      <c r="SO4" s="0"/>
+      <c r="SP4" s="0"/>
+      <c r="SQ4" s="0"/>
+      <c r="SR4" s="0"/>
+      <c r="SS4" s="0"/>
+      <c r="ST4" s="0"/>
+      <c r="SU4" s="0"/>
+      <c r="SV4" s="0"/>
+      <c r="SW4" s="0"/>
+      <c r="SX4" s="0"/>
+      <c r="SY4" s="0"/>
+      <c r="SZ4" s="0"/>
+      <c r="TA4" s="0"/>
+      <c r="TB4" s="0"/>
+      <c r="TC4" s="0"/>
+      <c r="TD4" s="0"/>
+      <c r="TE4" s="0"/>
+      <c r="TF4" s="0"/>
+      <c r="TG4" s="0"/>
+      <c r="TH4" s="0"/>
+      <c r="TI4" s="0"/>
+      <c r="TJ4" s="0"/>
+      <c r="TK4" s="0"/>
+      <c r="TL4" s="0"/>
+      <c r="TM4" s="0"/>
+      <c r="TN4" s="0"/>
+      <c r="TO4" s="0"/>
+      <c r="TP4" s="0"/>
+      <c r="TQ4" s="0"/>
+      <c r="TR4" s="0"/>
+      <c r="TS4" s="0"/>
+      <c r="TT4" s="0"/>
+      <c r="TU4" s="0"/>
+      <c r="TV4" s="0"/>
+      <c r="TW4" s="0"/>
+      <c r="TX4" s="0"/>
+      <c r="TY4" s="0"/>
+      <c r="TZ4" s="0"/>
+      <c r="UA4" s="0"/>
+      <c r="UB4" s="0"/>
+      <c r="UC4" s="0"/>
+      <c r="UD4" s="0"/>
+      <c r="UE4" s="0"/>
+      <c r="UF4" s="0"/>
+      <c r="UG4" s="0"/>
+      <c r="UH4" s="0"/>
+      <c r="UI4" s="0"/>
+      <c r="UJ4" s="0"/>
+      <c r="UK4" s="0"/>
+      <c r="UL4" s="0"/>
+      <c r="UM4" s="0"/>
+      <c r="UN4" s="0"/>
+      <c r="UO4" s="0"/>
+      <c r="UP4" s="0"/>
+      <c r="UQ4" s="0"/>
+      <c r="UR4" s="0"/>
+      <c r="US4" s="0"/>
+      <c r="UT4" s="0"/>
+      <c r="UU4" s="0"/>
+      <c r="UV4" s="0"/>
+      <c r="UW4" s="0"/>
+      <c r="UX4" s="0"/>
+      <c r="UY4" s="0"/>
+      <c r="UZ4" s="0"/>
+      <c r="VA4" s="0"/>
+      <c r="VB4" s="0"/>
+      <c r="VC4" s="0"/>
+      <c r="VD4" s="0"/>
+      <c r="VE4" s="0"/>
+      <c r="VF4" s="0"/>
+      <c r="VG4" s="0"/>
+      <c r="VH4" s="0"/>
+      <c r="VI4" s="0"/>
+      <c r="VJ4" s="0"/>
+      <c r="VK4" s="0"/>
+      <c r="VL4" s="0"/>
+      <c r="VM4" s="0"/>
+      <c r="VN4" s="0"/>
+      <c r="VO4" s="0"/>
+      <c r="VP4" s="0"/>
+      <c r="VQ4" s="0"/>
+      <c r="VR4" s="0"/>
+      <c r="VS4" s="0"/>
+      <c r="VT4" s="0"/>
+      <c r="VU4" s="0"/>
+      <c r="VV4" s="0"/>
+      <c r="VW4" s="0"/>
+      <c r="VX4" s="0"/>
+      <c r="VY4" s="0"/>
+      <c r="VZ4" s="0"/>
+      <c r="WA4" s="0"/>
+      <c r="WB4" s="0"/>
+      <c r="WC4" s="0"/>
+      <c r="WD4" s="0"/>
+      <c r="WE4" s="0"/>
+      <c r="WF4" s="0"/>
+      <c r="WG4" s="0"/>
+      <c r="WH4" s="0"/>
+      <c r="WI4" s="0"/>
+      <c r="WJ4" s="0"/>
+      <c r="WK4" s="0"/>
+      <c r="WL4" s="0"/>
+      <c r="WM4" s="0"/>
+      <c r="WN4" s="0"/>
+      <c r="WO4" s="0"/>
+      <c r="WP4" s="0"/>
+      <c r="WQ4" s="0"/>
+      <c r="WR4" s="0"/>
+      <c r="WS4" s="0"/>
+      <c r="WT4" s="0"/>
+      <c r="WU4" s="0"/>
+      <c r="WV4" s="0"/>
+      <c r="WW4" s="0"/>
+      <c r="WX4" s="0"/>
+      <c r="WY4" s="0"/>
+      <c r="WZ4" s="0"/>
+      <c r="XA4" s="0"/>
+      <c r="XB4" s="0"/>
+      <c r="XC4" s="0"/>
+      <c r="XD4" s="0"/>
+      <c r="XE4" s="0"/>
+      <c r="XF4" s="0"/>
+      <c r="XG4" s="0"/>
+      <c r="XH4" s="0"/>
+      <c r="XI4" s="0"/>
+      <c r="XJ4" s="0"/>
+      <c r="XK4" s="0"/>
+      <c r="XL4" s="0"/>
+      <c r="XM4" s="0"/>
+      <c r="XN4" s="0"/>
+      <c r="XO4" s="0"/>
+      <c r="XP4" s="0"/>
+      <c r="XQ4" s="0"/>
+      <c r="XR4" s="0"/>
+      <c r="XS4" s="0"/>
+      <c r="XT4" s="0"/>
+      <c r="XU4" s="0"/>
+      <c r="XV4" s="0"/>
+      <c r="XW4" s="0"/>
+      <c r="XX4" s="0"/>
+      <c r="XY4" s="0"/>
+      <c r="XZ4" s="0"/>
+      <c r="YA4" s="0"/>
+      <c r="YB4" s="0"/>
+      <c r="YC4" s="0"/>
+      <c r="YD4" s="0"/>
+      <c r="YE4" s="0"/>
+      <c r="YF4" s="0"/>
+      <c r="YG4" s="0"/>
+      <c r="YH4" s="0"/>
+      <c r="YI4" s="0"/>
+      <c r="YJ4" s="0"/>
+      <c r="YK4" s="0"/>
+      <c r="YL4" s="0"/>
+      <c r="YM4" s="0"/>
+      <c r="YN4" s="0"/>
+      <c r="YO4" s="0"/>
+      <c r="YP4" s="0"/>
+      <c r="YQ4" s="0"/>
+      <c r="YR4" s="0"/>
+      <c r="YS4" s="0"/>
+      <c r="YT4" s="0"/>
+      <c r="YU4" s="0"/>
+      <c r="YV4" s="0"/>
+      <c r="YW4" s="0"/>
+      <c r="YX4" s="0"/>
+      <c r="YY4" s="0"/>
+      <c r="YZ4" s="0"/>
+      <c r="ZA4" s="0"/>
+      <c r="ZB4" s="0"/>
+      <c r="ZC4" s="0"/>
+      <c r="ZD4" s="0"/>
+      <c r="ZE4" s="0"/>
+      <c r="ZF4" s="0"/>
+      <c r="ZG4" s="0"/>
+      <c r="ZH4" s="0"/>
+      <c r="ZI4" s="0"/>
+      <c r="ZJ4" s="0"/>
+      <c r="ZK4" s="0"/>
+      <c r="ZL4" s="0"/>
+      <c r="ZM4" s="0"/>
+      <c r="ZN4" s="0"/>
+      <c r="ZO4" s="0"/>
+      <c r="ZP4" s="0"/>
+      <c r="ZQ4" s="0"/>
+      <c r="ZR4" s="0"/>
+      <c r="ZS4" s="0"/>
+      <c r="ZT4" s="0"/>
+      <c r="ZU4" s="0"/>
+      <c r="ZV4" s="0"/>
+      <c r="ZW4" s="0"/>
+      <c r="ZX4" s="0"/>
+      <c r="ZY4" s="0"/>
+      <c r="ZZ4" s="0"/>
+      <c r="AAA4" s="0"/>
+      <c r="AAB4" s="0"/>
+      <c r="AAC4" s="0"/>
+      <c r="AAD4" s="0"/>
+      <c r="AAE4" s="0"/>
+      <c r="AAF4" s="0"/>
+      <c r="AAG4" s="0"/>
+      <c r="AAH4" s="0"/>
+      <c r="AAI4" s="0"/>
+      <c r="AAJ4" s="0"/>
+      <c r="AAK4" s="0"/>
+      <c r="AAL4" s="0"/>
+      <c r="AAM4" s="0"/>
+      <c r="AAN4" s="0"/>
+      <c r="AAO4" s="0"/>
+      <c r="AAP4" s="0"/>
+      <c r="AAQ4" s="0"/>
+      <c r="AAR4" s="0"/>
+      <c r="AAS4" s="0"/>
+      <c r="AAT4" s="0"/>
+      <c r="AAU4" s="0"/>
+      <c r="AAV4" s="0"/>
+      <c r="AAW4" s="0"/>
+      <c r="AAX4" s="0"/>
+      <c r="AAY4" s="0"/>
+      <c r="AAZ4" s="0"/>
+      <c r="ABA4" s="0"/>
+      <c r="ABB4" s="0"/>
+      <c r="ABC4" s="0"/>
+      <c r="ABD4" s="0"/>
+      <c r="ABE4" s="0"/>
+      <c r="ABF4" s="0"/>
+      <c r="ABG4" s="0"/>
+      <c r="ABH4" s="0"/>
+      <c r="ABI4" s="0"/>
+      <c r="ABJ4" s="0"/>
+      <c r="ABK4" s="0"/>
+      <c r="ABL4" s="0"/>
+      <c r="ABM4" s="0"/>
+      <c r="ABN4" s="0"/>
+      <c r="ABO4" s="0"/>
+      <c r="ABP4" s="0"/>
+      <c r="ABQ4" s="0"/>
+      <c r="ABR4" s="0"/>
+      <c r="ABS4" s="0"/>
+      <c r="ABT4" s="0"/>
+      <c r="ABU4" s="0"/>
+      <c r="ABV4" s="0"/>
+      <c r="ABW4" s="0"/>
+      <c r="ABX4" s="0"/>
+      <c r="ABY4" s="0"/>
+      <c r="ABZ4" s="0"/>
+      <c r="ACA4" s="0"/>
+      <c r="ACB4" s="0"/>
+      <c r="ACC4" s="0"/>
+      <c r="ACD4" s="0"/>
+      <c r="ACE4" s="0"/>
+      <c r="ACF4" s="0"/>
+      <c r="ACG4" s="0"/>
+      <c r="ACH4" s="0"/>
+      <c r="ACI4" s="0"/>
+      <c r="ACJ4" s="0"/>
+      <c r="ACK4" s="0"/>
+      <c r="ACL4" s="0"/>
+      <c r="ACM4" s="0"/>
+      <c r="ACN4" s="0"/>
+      <c r="ACO4" s="0"/>
+      <c r="ACP4" s="0"/>
+      <c r="ACQ4" s="0"/>
+      <c r="ACR4" s="0"/>
+      <c r="ACS4" s="0"/>
+      <c r="ACT4" s="0"/>
+      <c r="ACU4" s="0"/>
+      <c r="ACV4" s="0"/>
+      <c r="ACW4" s="0"/>
+      <c r="ACX4" s="0"/>
+      <c r="ACY4" s="0"/>
+      <c r="ACZ4" s="0"/>
+      <c r="ADA4" s="0"/>
+      <c r="ADB4" s="0"/>
+      <c r="ADC4" s="0"/>
+      <c r="ADD4" s="0"/>
+      <c r="ADE4" s="0"/>
+      <c r="ADF4" s="0"/>
+      <c r="ADG4" s="0"/>
+      <c r="ADH4" s="0"/>
+      <c r="ADI4" s="0"/>
+      <c r="ADJ4" s="0"/>
+      <c r="ADK4" s="0"/>
+      <c r="ADL4" s="0"/>
+      <c r="ADM4" s="0"/>
+      <c r="ADN4" s="0"/>
+      <c r="ADO4" s="0"/>
+      <c r="ADP4" s="0"/>
+      <c r="ADQ4" s="0"/>
+      <c r="ADR4" s="0"/>
+      <c r="ADS4" s="0"/>
+      <c r="ADT4" s="0"/>
+      <c r="ADU4" s="0"/>
+      <c r="ADV4" s="0"/>
+      <c r="ADW4" s="0"/>
+      <c r="ADX4" s="0"/>
+      <c r="ADY4" s="0"/>
+      <c r="ADZ4" s="0"/>
+      <c r="AEA4" s="0"/>
+      <c r="AEB4" s="0"/>
+      <c r="AEC4" s="0"/>
+      <c r="AED4" s="0"/>
+      <c r="AEE4" s="0"/>
+      <c r="AEF4" s="0"/>
+      <c r="AEG4" s="0"/>
+      <c r="AEH4" s="0"/>
+      <c r="AEI4" s="0"/>
+      <c r="AEJ4" s="0"/>
+      <c r="AEK4" s="0"/>
+      <c r="AEL4" s="0"/>
+      <c r="AEM4" s="0"/>
+      <c r="AEN4" s="0"/>
+      <c r="AEO4" s="0"/>
+      <c r="AEP4" s="0"/>
+      <c r="AEQ4" s="0"/>
+      <c r="AER4" s="0"/>
+      <c r="AES4" s="0"/>
+      <c r="AET4" s="0"/>
+      <c r="AEU4" s="0"/>
+      <c r="AEV4" s="0"/>
+      <c r="AEW4" s="0"/>
+      <c r="AEX4" s="0"/>
+      <c r="AEY4" s="0"/>
+      <c r="AEZ4" s="0"/>
+      <c r="AFA4" s="0"/>
+      <c r="AFB4" s="0"/>
+      <c r="AFC4" s="0"/>
+      <c r="AFD4" s="0"/>
+      <c r="AFE4" s="0"/>
+      <c r="AFF4" s="0"/>
+      <c r="AFG4" s="0"/>
+      <c r="AFH4" s="0"/>
+      <c r="AFI4" s="0"/>
+      <c r="AFJ4" s="0"/>
+      <c r="AFK4" s="0"/>
+      <c r="AFL4" s="0"/>
+      <c r="AFM4" s="0"/>
+      <c r="AFN4" s="0"/>
+      <c r="AFO4" s="0"/>
+      <c r="AFP4" s="0"/>
+      <c r="AFQ4" s="0"/>
+      <c r="AFR4" s="0"/>
+      <c r="AFS4" s="0"/>
+      <c r="AFT4" s="0"/>
+      <c r="AFU4" s="0"/>
+      <c r="AFV4" s="0"/>
+      <c r="AFW4" s="0"/>
+      <c r="AFX4" s="0"/>
+      <c r="AFY4" s="0"/>
+      <c r="AFZ4" s="0"/>
+      <c r="AGA4" s="0"/>
+      <c r="AGB4" s="0"/>
+      <c r="AGC4" s="0"/>
+      <c r="AGD4" s="0"/>
+      <c r="AGE4" s="0"/>
+      <c r="AGF4" s="0"/>
+      <c r="AGG4" s="0"/>
+      <c r="AGH4" s="0"/>
+      <c r="AGI4" s="0"/>
+      <c r="AGJ4" s="0"/>
+      <c r="AGK4" s="0"/>
+      <c r="AGL4" s="0"/>
+      <c r="AGM4" s="0"/>
+      <c r="AGN4" s="0"/>
+      <c r="AGO4" s="0"/>
+      <c r="AGP4" s="0"/>
+      <c r="AGQ4" s="0"/>
+      <c r="AGR4" s="0"/>
+      <c r="AGS4" s="0"/>
+      <c r="AGT4" s="0"/>
+      <c r="AGU4" s="0"/>
+      <c r="AGV4" s="0"/>
+      <c r="AGW4" s="0"/>
+      <c r="AGX4" s="0"/>
+      <c r="AGY4" s="0"/>
+      <c r="AGZ4" s="0"/>
+      <c r="AHA4" s="0"/>
+      <c r="AHB4" s="0"/>
+      <c r="AHC4" s="0"/>
+      <c r="AHD4" s="0"/>
+      <c r="AHE4" s="0"/>
+      <c r="AHF4" s="0"/>
+      <c r="AHG4" s="0"/>
+      <c r="AHH4" s="0"/>
+      <c r="AHI4" s="0"/>
+      <c r="AHJ4" s="0"/>
+      <c r="AHK4" s="0"/>
+      <c r="AHL4" s="0"/>
+      <c r="AHM4" s="0"/>
+      <c r="AHN4" s="0"/>
+      <c r="AHO4" s="0"/>
+      <c r="AHP4" s="0"/>
+      <c r="AHQ4" s="0"/>
+      <c r="AHR4" s="0"/>
+      <c r="AHS4" s="0"/>
+      <c r="AHT4" s="0"/>
+      <c r="AHU4" s="0"/>
+      <c r="AHV4" s="0"/>
+      <c r="AHW4" s="0"/>
+      <c r="AHX4" s="0"/>
+      <c r="AHY4" s="0"/>
+      <c r="AHZ4" s="0"/>
+      <c r="AIA4" s="0"/>
+      <c r="AIB4" s="0"/>
+      <c r="AIC4" s="0"/>
+      <c r="AID4" s="0"/>
+      <c r="AIE4" s="0"/>
+      <c r="AIF4" s="0"/>
+      <c r="AIG4" s="0"/>
+      <c r="AIH4" s="0"/>
+      <c r="AII4" s="0"/>
+      <c r="AIJ4" s="0"/>
+      <c r="AIK4" s="0"/>
+      <c r="AIL4" s="0"/>
+      <c r="AIM4" s="0"/>
+      <c r="AIN4" s="0"/>
+      <c r="AIO4" s="0"/>
+      <c r="AIP4" s="0"/>
+      <c r="AIQ4" s="0"/>
+      <c r="AIR4" s="0"/>
+      <c r="AIS4" s="0"/>
+      <c r="AIT4" s="0"/>
+      <c r="AIU4" s="0"/>
+      <c r="AIV4" s="0"/>
+      <c r="AIW4" s="0"/>
+      <c r="AIX4" s="0"/>
+      <c r="AIY4" s="0"/>
+      <c r="AIZ4" s="0"/>
+      <c r="AJA4" s="0"/>
+      <c r="AJB4" s="0"/>
+      <c r="AJC4" s="0"/>
+      <c r="AJD4" s="0"/>
+      <c r="AJE4" s="0"/>
+      <c r="AJF4" s="0"/>
+      <c r="AJG4" s="0"/>
+      <c r="AJH4" s="0"/>
+      <c r="AJI4" s="0"/>
+      <c r="AJJ4" s="0"/>
+      <c r="AJK4" s="0"/>
+      <c r="AJL4" s="0"/>
+      <c r="AJM4" s="0"/>
+      <c r="AJN4" s="0"/>
+      <c r="AJO4" s="0"/>
+      <c r="AJP4" s="0"/>
+      <c r="AJQ4" s="0"/>
+      <c r="AJR4" s="0"/>
+      <c r="AJS4" s="0"/>
+      <c r="AJT4" s="0"/>
+      <c r="AJU4" s="0"/>
+      <c r="AJV4" s="0"/>
+      <c r="AJW4" s="0"/>
+      <c r="AJX4" s="0"/>
+      <c r="AJY4" s="0"/>
+      <c r="AJZ4" s="0"/>
+      <c r="AKA4" s="0"/>
+      <c r="AKB4" s="0"/>
+      <c r="AKC4" s="0"/>
+      <c r="AKD4" s="0"/>
+      <c r="AKE4" s="0"/>
+      <c r="AKF4" s="0"/>
+      <c r="AKG4" s="0"/>
+      <c r="AKH4" s="0"/>
+      <c r="AKI4" s="0"/>
+      <c r="AKJ4" s="0"/>
+      <c r="AKK4" s="0"/>
+      <c r="AKL4" s="0"/>
+      <c r="AKM4" s="0"/>
+      <c r="AKN4" s="0"/>
+      <c r="AKO4" s="0"/>
+      <c r="AKP4" s="0"/>
+      <c r="AKQ4" s="0"/>
+      <c r="AKR4" s="0"/>
+      <c r="AKS4" s="0"/>
+      <c r="AKT4" s="0"/>
+      <c r="AKU4" s="0"/>
+      <c r="AKV4" s="0"/>
+      <c r="AKW4" s="0"/>
+      <c r="AKX4" s="0"/>
+      <c r="AKY4" s="0"/>
+      <c r="AKZ4" s="0"/>
+      <c r="ALA4" s="0"/>
+      <c r="ALB4" s="0"/>
+      <c r="ALC4" s="0"/>
+      <c r="ALD4" s="0"/>
+      <c r="ALE4" s="0"/>
+      <c r="ALF4" s="0"/>
+      <c r="ALG4" s="0"/>
+      <c r="ALH4" s="0"/>
+      <c r="ALI4" s="0"/>
+      <c r="ALJ4" s="0"/>
+      <c r="ALK4" s="0"/>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
+      <c r="AMC4" s="0"/>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>33</v>
+      <c r="N5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="F6" s="13" t="s">
         <v>36</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="14"/>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>29</v>
+      <c r="N8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="6" t="s">
+      <c r="N9" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="F10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="M10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>29</v>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="M11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N11" s="15" t="s">
-        <v>36</v>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4066,271 +5119,1307 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="61.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="22.6224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="23.4591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="22.3826530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="26.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="16" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+    <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>46</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
       <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23" t="n">
+      <c r="B4" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="23" t="n">
+      <c r="C4" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="23" t="n">
+      <c r="D5" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="23" t="n">
+      <c r="E5" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="23" t="n">
+      <c r="C6" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="23" t="n">
+      <c r="E6" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="23" t="n">
+      <c r="C7" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="n">
+      <c r="D7" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="23" t="n">
+      <c r="E7" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="23" t="n">
+      <c r="C8" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="23" t="n">
+      <c r="D8" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="23" t="n">
+      <c r="E8" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="25"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="23" t="n">
+      <c r="C9" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="23" t="n">
+      <c r="D9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="23" t="n">
+      <c r="E9" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="23" t="n">
+      <c r="D10" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="23" t="n">
+      <c r="E10" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="23" t="n">
+      <c r="A11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="23" t="n">
+      <c r="D11" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="23" t="n">
+      <c r="E11" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>